<commit_message>
Replaced old charger to support JLC assembly. Very close now!
</commit_message>
<xml_diff>
--- a/Cost_JLC.xlsx
+++ b/Cost_JLC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaa bbb\Documents\KiCadProj\SmartBattery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB8F1F0-AA77-45D1-BC5D-EC1908E6F2B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776B6949-A16B-4B7D-AE9B-2F2150A63215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="3000" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost_Seeed" sheetId="1" r:id="rId1"/>
@@ -1394,7 +1394,7 @@
   <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>